<commit_message>
Fvk 2023 q2 update mortality (#326)
* fix devcontainer build and test workflow to have mc

* updated source from WS
</commit_message>
<xml_diff>
--- a/resources/quality_of_life/health_mortality/DOHMH_death rate and overdose.xlsx
+++ b/resources/quality_of_life/health_mortality/DOHMH_death rate and overdose.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nycdohmh-my.sharepoint.com/personal/wli_health_nyc_gov/Documents/Data Request/Deputy Commissioner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\EPI\VS\BVS\SA\SA-WR-Ying\NYS COVID Data Sharing daily dataset\mmmmmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C86BABA7-55C0-407F-A108-9EA39A0561B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDA716D-B43F-457F-91F9-FC8EBFDE7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="315">
   <si>
     <t>infant_mortality_per1000_2000</t>
   </si>
@@ -978,6 +978,9 @@
   </si>
   <si>
     <t>Unintentional overdose deaths involving any drug among NYC residents age 15-84 per 100,000 people in the years 2016-2020 to White non-Hispanic persons</t>
+  </si>
+  <si>
+    <t>Unintentional overdose deaths involving any drug among NYC residents age 15-84 per 100,000 people in the years 2010-2014  to all persons</t>
   </si>
 </sst>
 </file>
@@ -3115,11 +3118,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90DA47D-79FC-40F4-9A38-414CBAA5473A}">
-  <dimension ref="A1:AS63"/>
+  <dimension ref="A1:AT63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C21" sqref="C21"/>
+      <selection pane="topRight" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,16 +3163,16 @@
     <col min="37" max="37" width="38.85546875" style="43" customWidth="1"/>
     <col min="38" max="38" width="36.85546875" style="43" customWidth="1"/>
     <col min="39" max="39" width="37.5703125" style="43" customWidth="1"/>
-    <col min="40" max="40" width="37.7109375" style="43" customWidth="1"/>
-    <col min="41" max="41" width="39.5703125" style="54" customWidth="1"/>
-    <col min="42" max="42" width="36.85546875" style="54" customWidth="1"/>
-    <col min="43" max="43" width="37.5703125" style="54" customWidth="1"/>
-    <col min="44" max="44" width="36.85546875" style="54" customWidth="1"/>
-    <col min="45" max="45" width="35.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="17"/>
+    <col min="40" max="41" width="37.7109375" style="43" customWidth="1"/>
+    <col min="42" max="42" width="39.5703125" style="54" customWidth="1"/>
+    <col min="43" max="43" width="36.85546875" style="54" customWidth="1"/>
+    <col min="44" max="44" width="37.5703125" style="54" customWidth="1"/>
+    <col min="45" max="45" width="36.85546875" style="54" customWidth="1"/>
+    <col min="46" max="46" width="35.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>248</v>
       </c>
@@ -3287,23 +3290,26 @@
       <c r="AN1" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="AO1" s="52" t="s">
+      <c r="AO1" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="AP1" s="52" t="s">
         <v>313</v>
       </c>
-      <c r="AP1" s="52" t="s">
+      <c r="AQ1" s="52" t="s">
         <v>312</v>
       </c>
-      <c r="AQ1" s="52" t="s">
+      <c r="AR1" s="52" t="s">
         <v>311</v>
       </c>
-      <c r="AR1" s="52" t="s">
+      <c r="AS1" s="52" t="s">
         <v>310</v>
       </c>
-      <c r="AS1" s="52" t="s">
+      <c r="AT1" s="52" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>203</v>
       </c>
@@ -3424,23 +3430,26 @@
       <c r="AN2" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="AO2" s="53" t="s">
+      <c r="AO2" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="AP2" s="53" t="s">
         <v>304</v>
       </c>
-      <c r="AP2" s="53" t="s">
+      <c r="AQ2" s="53" t="s">
         <v>305</v>
       </c>
-      <c r="AQ2" s="53" t="s">
+      <c r="AR2" s="53" t="s">
         <v>306</v>
       </c>
-      <c r="AR2" s="53" t="s">
+      <c r="AS2" s="53" t="s">
         <v>307</v>
       </c>
-      <c r="AS2" s="53" t="s">
+      <c r="AT2" s="53" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>157</v>
       </c>
@@ -3562,22 +3571,25 @@
         <v>64</v>
       </c>
       <c r="AO3" s="45">
+        <v>7.1421000000000001</v>
+      </c>
+      <c r="AP3" s="45">
         <v>21.5</v>
       </c>
-      <c r="AP3" s="45">
+      <c r="AQ3" s="45">
         <v>25.8</v>
       </c>
-      <c r="AQ3" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR3" s="45">
+      <c r="AR3" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS3" s="45">
         <v>18.3</v>
       </c>
-      <c r="AS3" s="45">
+      <c r="AT3" s="45">
         <v>18.5</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>156</v>
       </c>
@@ -3699,22 +3711,25 @@
         <v>64</v>
       </c>
       <c r="AO4" s="45">
+        <v>6.3003999999999998</v>
+      </c>
+      <c r="AP4" s="45">
         <v>58.5</v>
       </c>
-      <c r="AP4" s="45">
+      <c r="AQ4" s="45">
         <v>16.5</v>
       </c>
-      <c r="AQ4" s="45">
-        <v>0</v>
-      </c>
       <c r="AR4" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="45">
         <v>44.2</v>
       </c>
-      <c r="AS4" s="45">
+      <c r="AT4" s="45">
         <v>24.9</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>155</v>
       </c>
@@ -3836,22 +3851,25 @@
         <v>64</v>
       </c>
       <c r="AO5" s="45">
+        <v>9.4998000000000005</v>
+      </c>
+      <c r="AP5" s="45">
         <v>45.2</v>
       </c>
-      <c r="AP5" s="45">
+      <c r="AQ5" s="45">
         <v>12.1</v>
       </c>
-      <c r="AQ5" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR5" s="45">
+      <c r="AR5" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS5" s="45">
         <v>25.1</v>
       </c>
-      <c r="AS5" s="45">
+      <c r="AT5" s="45">
         <v>26.8</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>154</v>
       </c>
@@ -3973,22 +3991,25 @@
         <v>7.9</v>
       </c>
       <c r="AO6" s="45">
+        <v>9.4245000000000001</v>
+      </c>
+      <c r="AP6" s="45">
         <v>33.299999999999997</v>
       </c>
-      <c r="AP6" s="45">
+      <c r="AQ6" s="45">
         <v>18.3</v>
       </c>
-      <c r="AQ6" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR6" s="45">
+      <c r="AR6" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS6" s="45">
         <v>24</v>
       </c>
-      <c r="AS6" s="45">
+      <c r="AT6" s="45">
         <v>22.8</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>153</v>
       </c>
@@ -4110,22 +4131,25 @@
         <v>13.5</v>
       </c>
       <c r="AO7" s="45">
+        <v>16.691600000000001</v>
+      </c>
+      <c r="AP7" s="45">
         <v>167.5</v>
       </c>
-      <c r="AP7" s="45">
+      <c r="AQ7" s="45">
         <v>60.2</v>
       </c>
-      <c r="AQ7" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR7" s="45">
+      <c r="AR7" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS7" s="45">
         <v>38.6</v>
       </c>
-      <c r="AS7" s="45">
+      <c r="AT7" s="45">
         <v>49.2</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>152</v>
       </c>
@@ -4247,22 +4271,25 @@
         <v>11.6</v>
       </c>
       <c r="AO8" s="45">
+        <v>11.1823</v>
+      </c>
+      <c r="AP8" s="45">
         <v>86.6</v>
       </c>
-      <c r="AP8" s="45">
+      <c r="AQ8" s="45">
         <v>40</v>
       </c>
-      <c r="AQ8" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR8" s="45">
+      <c r="AR8" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS8" s="45">
         <v>33.9</v>
       </c>
-      <c r="AS8" s="45">
+      <c r="AT8" s="45">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>151</v>
       </c>
@@ -4384,22 +4411,25 @@
         <v>9</v>
       </c>
       <c r="AO9" s="45">
+        <v>9.6609999999999996</v>
+      </c>
+      <c r="AP9" s="45">
         <v>343</v>
       </c>
-      <c r="AP9" s="45">
+      <c r="AQ9" s="45">
         <v>47.3</v>
       </c>
-      <c r="AQ9" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR9" s="45">
+      <c r="AR9" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS9" s="45">
         <v>36</v>
       </c>
-      <c r="AS9" s="45">
+      <c r="AT9" s="45">
         <v>43.5</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>150</v>
       </c>
@@ -4521,22 +4551,25 @@
         <v>11.9</v>
       </c>
       <c r="AO10" s="45">
+        <v>11.204000000000001</v>
+      </c>
+      <c r="AP10" s="45">
         <v>159.30000000000001</v>
       </c>
-      <c r="AP10" s="45">
+      <c r="AQ10" s="45">
         <v>38.6</v>
       </c>
-      <c r="AQ10" s="45">
-        <v>0</v>
-      </c>
       <c r="AR10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="45">
         <v>29.9</v>
       </c>
-      <c r="AS10" s="45">
+      <c r="AT10" s="45">
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
@@ -4658,22 +4691,25 @@
         <v>10.199999999999999</v>
       </c>
       <c r="AO11" s="45">
+        <v>9.0975000000000001</v>
+      </c>
+      <c r="AP11" s="45">
         <v>124</v>
       </c>
-      <c r="AP11" s="45">
+      <c r="AQ11" s="45">
         <v>21.9</v>
       </c>
-      <c r="AQ11" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR11" s="45">
+      <c r="AR11" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS11" s="45">
         <v>23.4</v>
       </c>
-      <c r="AS11" s="45">
+      <c r="AT11" s="45">
         <v>24.1</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>148</v>
       </c>
@@ -4795,22 +4831,25 @@
         <v>12.4</v>
       </c>
       <c r="AO12" s="45">
+        <v>17.1264</v>
+      </c>
+      <c r="AP12" s="45">
         <v>301.89999999999998</v>
       </c>
-      <c r="AP12" s="45">
+      <c r="AQ12" s="45">
         <v>70.099999999999994</v>
       </c>
-      <c r="AQ12" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR12" s="45">
+      <c r="AR12" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS12" s="45">
         <v>36.5</v>
       </c>
-      <c r="AS12" s="45">
+      <c r="AT12" s="45">
         <v>48.2</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>147</v>
       </c>
@@ -4932,22 +4971,25 @@
         <v>6</v>
       </c>
       <c r="AO13" s="45">
+        <v>7.8346999999999998</v>
+      </c>
+      <c r="AP13" s="45">
         <v>24.6</v>
       </c>
-      <c r="AP13" s="45">
+      <c r="AQ13" s="45">
         <v>39.299999999999997</v>
       </c>
-      <c r="AQ13" s="45">
-        <v>0</v>
-      </c>
       <c r="AR13" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="45">
         <v>20.399999999999999</v>
       </c>
-      <c r="AS13" s="45">
+      <c r="AT13" s="45">
         <v>22.1</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>146</v>
       </c>
@@ -5069,22 +5111,25 @@
         <v>64</v>
       </c>
       <c r="AO14" s="45">
+        <v>6.9358000000000004</v>
+      </c>
+      <c r="AP14" s="45">
         <v>31.6</v>
       </c>
-      <c r="AP14" s="45">
+      <c r="AQ14" s="45">
         <v>38.6</v>
       </c>
-      <c r="AQ14" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR14" s="45">
+      <c r="AR14" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS14" s="45">
         <v>25.3</v>
       </c>
-      <c r="AS14" s="45">
+      <c r="AT14" s="45">
         <v>29.4</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>145</v>
       </c>
@@ -5206,22 +5251,25 @@
         <v>64</v>
       </c>
       <c r="AO15" s="45">
+        <v>16.707999999999998</v>
+      </c>
+      <c r="AP15" s="45">
         <v>44.9</v>
       </c>
-      <c r="AP15" s="45">
+      <c r="AQ15" s="45">
         <v>36.6</v>
       </c>
-      <c r="AQ15" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR15" s="45">
+      <c r="AR15" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS15" s="45">
         <v>40.9</v>
       </c>
-      <c r="AS15" s="45">
+      <c r="AT15" s="45">
         <v>37.5</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>144</v>
       </c>
@@ -5343,22 +5391,25 @@
         <v>11.2</v>
       </c>
       <c r="AO16" s="45">
+        <v>15.3544</v>
+      </c>
+      <c r="AP16" s="45">
         <v>37</v>
       </c>
-      <c r="AP16" s="45">
+      <c r="AQ16" s="45">
         <v>48.1</v>
       </c>
-      <c r="AQ16" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR16" s="45">
+      <c r="AR16" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS16" s="45">
         <v>37.700000000000003</v>
       </c>
-      <c r="AS16" s="45">
+      <c r="AT16" s="45">
         <v>39.9</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>143</v>
       </c>
@@ -5480,22 +5531,25 @@
         <v>64</v>
       </c>
       <c r="AO17" s="45">
+        <v>5.1947999999999999</v>
+      </c>
+      <c r="AP17" s="45">
         <v>7.9</v>
       </c>
-      <c r="AP17" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ17" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS17" s="45">
+      <c r="AQ17" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR17" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT17" s="45">
         <v>7.7</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>142</v>
       </c>
@@ -5617,22 +5671,25 @@
         <v>64</v>
       </c>
       <c r="AO18" s="45">
+        <v>4.6740000000000004</v>
+      </c>
+      <c r="AP18" s="45">
         <v>8.4</v>
       </c>
-      <c r="AP18" s="45">
+      <c r="AQ18" s="45">
         <v>37.9</v>
       </c>
-      <c r="AQ18" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR18" s="45">
+      <c r="AR18" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS18" s="45">
         <v>22.7</v>
       </c>
-      <c r="AS18" s="45">
+      <c r="AT18" s="45">
         <v>12.5</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>141</v>
       </c>
@@ -5754,22 +5811,25 @@
         <v>64</v>
       </c>
       <c r="AO19" s="45">
+        <v>7.5799000000000003</v>
+      </c>
+      <c r="AP19" s="45">
         <v>13.6</v>
       </c>
-      <c r="AP19" s="45">
+      <c r="AQ19" s="45">
         <v>37.5</v>
       </c>
-      <c r="AQ19" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR19" s="45">
+      <c r="AR19" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS19" s="45">
         <v>22</v>
       </c>
-      <c r="AS19" s="45">
+      <c r="AT19" s="45">
         <v>15.5</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>140</v>
       </c>
@@ -5891,22 +5951,25 @@
         <v>64</v>
       </c>
       <c r="AO20" s="45">
+        <v>4.9225000000000003</v>
+      </c>
+      <c r="AP20" s="45">
         <v>10.1</v>
       </c>
-      <c r="AP20" s="45">
+      <c r="AQ20" s="45">
         <v>46.1</v>
       </c>
-      <c r="AQ20" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AR20" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS20" s="45">
+      <c r="AS20" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT20" s="45">
         <v>11.7</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>139</v>
       </c>
@@ -6028,22 +6091,25 @@
         <v>10.8</v>
       </c>
       <c r="AO21" s="45">
+        <v>10.283799999999999</v>
+      </c>
+      <c r="AP21" s="45">
         <v>28.8</v>
       </c>
-      <c r="AP21" s="45">
+      <c r="AQ21" s="45">
         <v>61.7</v>
       </c>
-      <c r="AQ21" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR21" s="45">
+      <c r="AR21" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS21" s="45">
         <v>43.1</v>
       </c>
-      <c r="AS21" s="45">
+      <c r="AT21" s="45">
         <v>23.8</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>138</v>
       </c>
@@ -6165,22 +6231,25 @@
         <v>64</v>
       </c>
       <c r="AO22" s="45">
+        <v>5.2385999999999999</v>
+      </c>
+      <c r="AP22" s="45">
         <v>6</v>
       </c>
-      <c r="AP22" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ22" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR22" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS22" s="45">
+      <c r="AQ22" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR22" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT22" s="45">
         <v>6.2</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>137</v>
       </c>
@@ -6302,22 +6371,25 @@
         <v>64</v>
       </c>
       <c r="AO23" s="45">
+        <v>19.974</v>
+      </c>
+      <c r="AP23" s="45">
         <v>37</v>
       </c>
-      <c r="AP23" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ23" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR23" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS23" s="45">
+      <c r="AQ23" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR23" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS23" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT23" s="45">
         <v>31.9</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>136</v>
       </c>
@@ -6439,22 +6511,25 @@
         <v>64</v>
       </c>
       <c r="AO24" s="45">
+        <v>18.209099999999999</v>
+      </c>
+      <c r="AP24" s="45">
         <v>34.299999999999997</v>
       </c>
-      <c r="AP24" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ24" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR24" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS24" s="45">
+      <c r="AS24" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT24" s="45">
         <v>26.3</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>135</v>
       </c>
@@ -6576,22 +6651,25 @@
         <v>10.1</v>
       </c>
       <c r="AO25" s="45">
+        <v>15.126899999999999</v>
+      </c>
+      <c r="AP25" s="45">
         <v>47.1</v>
       </c>
-      <c r="AP25" s="45">
+      <c r="AQ25" s="45">
         <v>25.2</v>
       </c>
-      <c r="AQ25" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR25" s="45">
+      <c r="AR25" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS25" s="45">
         <v>23.5</v>
       </c>
-      <c r="AS25" s="45">
+      <c r="AT25" s="45">
         <v>30.7</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>134</v>
       </c>
@@ -6713,22 +6791,25 @@
         <v>14.1</v>
       </c>
       <c r="AO26" s="45">
+        <v>10.9465</v>
+      </c>
+      <c r="AP26" s="45">
         <v>14.4</v>
       </c>
-      <c r="AP26" s="45">
+      <c r="AQ26" s="45">
         <v>41.4</v>
       </c>
-      <c r="AQ26" s="45">
-        <v>0</v>
-      </c>
       <c r="AR26" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS26" s="45">
         <v>22.5</v>
       </c>
-      <c r="AS26" s="45">
+      <c r="AT26" s="45">
         <v>18.2</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>133</v>
       </c>
@@ -6849,23 +6930,26 @@
       <c r="AN27" s="45">
         <v>8.6</v>
       </c>
-      <c r="AO27" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP27" s="45">
+      <c r="AO27" s="45">
+        <v>11.054399999999999</v>
+      </c>
+      <c r="AP27" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ27" s="45">
         <v>28</v>
       </c>
-      <c r="AQ27" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR27" s="45">
+      <c r="AR27" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS27" s="45">
         <v>11.1</v>
       </c>
-      <c r="AS27" s="45">
+      <c r="AT27" s="45">
         <v>17.2</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>132</v>
       </c>
@@ -6986,23 +7070,26 @@
       <c r="AN28" s="45">
         <v>22.2</v>
       </c>
-      <c r="AO28" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP28" s="45">
+      <c r="AO28" s="45">
+        <v>14.3065</v>
+      </c>
+      <c r="AP28" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ28" s="45">
         <v>14.5</v>
       </c>
-      <c r="AQ28" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR28" s="45">
+      <c r="AR28" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS28" s="45">
         <v>37</v>
       </c>
-      <c r="AS28" s="45">
+      <c r="AT28" s="45">
         <v>21.2</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>131</v>
       </c>
@@ -7124,22 +7211,25 @@
         <v>64</v>
       </c>
       <c r="AO29" s="45">
+        <v>6.9512999999999998</v>
+      </c>
+      <c r="AP29" s="45">
         <v>7.4</v>
       </c>
-      <c r="AP29" s="45">
+      <c r="AQ29" s="45">
         <v>18.8</v>
       </c>
-      <c r="AQ29" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR29" s="45">
+      <c r="AR29" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS29" s="45">
         <v>23.8</v>
       </c>
-      <c r="AS29" s="45">
+      <c r="AT29" s="45">
         <v>13.5</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>130</v>
       </c>
@@ -7261,22 +7351,25 @@
         <v>64</v>
       </c>
       <c r="AO30" s="45">
+        <v>7.8324999999999996</v>
+      </c>
+      <c r="AP30" s="45">
         <v>6.9</v>
       </c>
-      <c r="AP30" s="45">
+      <c r="AQ30" s="45">
         <v>30.9</v>
       </c>
-      <c r="AQ30" s="45">
-        <v>0</v>
-      </c>
       <c r="AR30" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="45">
         <v>27.2</v>
       </c>
-      <c r="AS30" s="45">
+      <c r="AT30" s="45">
         <v>13.3</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>129</v>
       </c>
@@ -7398,22 +7491,25 @@
         <v>64</v>
       </c>
       <c r="AO31" s="45">
+        <v>9.8009000000000004</v>
+      </c>
+      <c r="AP31" s="45">
         <v>24.6</v>
       </c>
-      <c r="AP31" s="45">
+      <c r="AQ31" s="45">
         <v>15.2</v>
       </c>
-      <c r="AQ31" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AR31" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS31" s="45">
+      <c r="AS31" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT31" s="45">
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>128</v>
       </c>
@@ -7535,22 +7631,25 @@
         <v>21.3</v>
       </c>
       <c r="AO32" s="45">
+        <v>20.173100000000002</v>
+      </c>
+      <c r="AP32" s="45">
         <v>417.1</v>
       </c>
-      <c r="AP32" s="45">
+      <c r="AQ32" s="45">
         <v>22.8</v>
       </c>
-      <c r="AQ32" s="45">
-        <v>0</v>
-      </c>
       <c r="AR32" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="45">
         <v>45.1</v>
       </c>
-      <c r="AS32" s="45">
+      <c r="AT32" s="45">
         <v>31.9</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>127</v>
       </c>
@@ -7672,22 +7771,25 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="AO33" s="45">
+        <v>9.2443000000000008</v>
+      </c>
+      <c r="AP33" s="45">
         <v>91.9</v>
       </c>
-      <c r="AP33" s="45">
+      <c r="AQ33" s="45">
         <v>28.8</v>
       </c>
-      <c r="AQ33" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR33" s="45">
+      <c r="AR33" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS33" s="45">
         <v>21.8</v>
       </c>
-      <c r="AS33" s="45">
+      <c r="AT33" s="45">
         <v>26.5</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>126</v>
       </c>
@@ -7809,22 +7911,25 @@
         <v>64</v>
       </c>
       <c r="AO34" s="45">
+        <v>6.75</v>
+      </c>
+      <c r="AP34" s="45">
         <v>23.4</v>
       </c>
-      <c r="AP34" s="45">
+      <c r="AQ34" s="45">
         <v>5.6</v>
       </c>
-      <c r="AQ34" s="45">
-        <v>0</v>
-      </c>
       <c r="AR34" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS34" s="45">
         <v>22.8</v>
       </c>
-      <c r="AS34" s="45">
+      <c r="AT34" s="45">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>125</v>
       </c>
@@ -7946,22 +8051,25 @@
         <v>64</v>
       </c>
       <c r="AO35" s="45">
+        <v>3.9531999999999998</v>
+      </c>
+      <c r="AP35" s="45">
         <v>132.1</v>
       </c>
-      <c r="AP35" s="45">
+      <c r="AQ35" s="45">
         <v>8.1</v>
       </c>
-      <c r="AQ35" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AR35" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS35" s="45">
+      <c r="AS35" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT35" s="45">
         <v>11.2</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>124</v>
       </c>
@@ -8083,22 +8191,25 @@
         <v>64</v>
       </c>
       <c r="AO36" s="45">
+        <v>4.7359999999999998</v>
+      </c>
+      <c r="AP36" s="45">
         <v>26.4</v>
       </c>
-      <c r="AP36" s="45">
+      <c r="AQ36" s="45">
         <v>11.6</v>
       </c>
-      <c r="AQ36" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR36" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS36" s="45">
+      <c r="AR36" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS36" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT36" s="45">
         <v>14.5</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>123</v>
       </c>
@@ -8220,22 +8331,25 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="AO37" s="45">
+        <v>6.9833999999999996</v>
+      </c>
+      <c r="AP37" s="45">
         <v>16.2</v>
       </c>
-      <c r="AP37" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ37" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR37" s="45">
+      <c r="AR37" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS37" s="45">
         <v>15.4</v>
       </c>
-      <c r="AS37" s="45">
+      <c r="AT37" s="45">
         <v>11.6</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>122</v>
       </c>
@@ -8357,22 +8471,25 @@
         <v>64</v>
       </c>
       <c r="AO38" s="45">
+        <v>11.797000000000001</v>
+      </c>
+      <c r="AP38" s="45">
         <v>19.8</v>
       </c>
-      <c r="AP38" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ38" s="45" t="s">
-        <v>64</v>
+      <c r="AQ38" s="45">
+        <v>0</v>
       </c>
       <c r="AR38" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS38" s="45">
+      <c r="AS38" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT38" s="45">
         <v>13.4</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>121</v>
       </c>
@@ -8494,22 +8611,25 @@
         <v>64</v>
       </c>
       <c r="AO39" s="45">
+        <v>3.0386000000000002</v>
+      </c>
+      <c r="AP39" s="45">
         <v>7.1</v>
       </c>
-      <c r="AP39" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ39" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR39" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS39" s="45">
+      <c r="AS39" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT39" s="45">
         <v>6.1</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>120</v>
       </c>
@@ -8631,22 +8751,25 @@
         <v>64</v>
       </c>
       <c r="AO40" s="45">
+        <v>5.0082000000000004</v>
+      </c>
+      <c r="AP40" s="45">
         <v>16.600000000000001</v>
       </c>
-      <c r="AP40" s="45">
+      <c r="AQ40" s="45">
         <v>6.8</v>
       </c>
-      <c r="AQ40" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR40" s="45">
+      <c r="AR40" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS40" s="45">
         <v>15.8</v>
       </c>
-      <c r="AS40" s="45">
+      <c r="AT40" s="45">
         <v>11.1</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>119</v>
       </c>
@@ -8768,22 +8891,25 @@
         <v>64</v>
       </c>
       <c r="AO41" s="45">
+        <v>7.9465000000000003</v>
+      </c>
+      <c r="AP41" s="45">
         <v>16.8</v>
       </c>
-      <c r="AP41" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ41" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR41" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS41" s="45">
+      <c r="AS41" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT41" s="45">
         <v>13.5</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>118</v>
       </c>
@@ -8905,22 +9031,25 @@
         <v>64</v>
       </c>
       <c r="AO42" s="45">
+        <v>6.9444999999999997</v>
+      </c>
+      <c r="AP42" s="45">
         <v>21.1</v>
       </c>
-      <c r="AP42" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ42" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR42" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS42" s="45">
+      <c r="AS42" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT42" s="45">
         <v>12.3</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>117</v>
       </c>
@@ -9042,22 +9171,25 @@
         <v>64</v>
       </c>
       <c r="AO43" s="45">
+        <v>14.154299999999999</v>
+      </c>
+      <c r="AP43" s="45">
         <v>32.6</v>
       </c>
-      <c r="AP43" s="45">
+      <c r="AQ43" s="45">
         <v>28.5</v>
       </c>
-      <c r="AQ43" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR43" s="45">
+      <c r="AR43" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS43" s="45">
         <v>19.399999999999999</v>
       </c>
-      <c r="AS43" s="45">
+      <c r="AT43" s="45">
         <v>23.6</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>116</v>
       </c>
@@ -9179,22 +9311,25 @@
         <v>5.9</v>
       </c>
       <c r="AO44" s="45">
+        <v>7.0617999999999999</v>
+      </c>
+      <c r="AP44" s="45">
         <v>17.8</v>
       </c>
-      <c r="AP44" s="45">
+      <c r="AQ44" s="45">
         <v>23.1</v>
       </c>
-      <c r="AQ44" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR44" s="45">
+      <c r="AR44" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS44" s="45">
         <v>12</v>
       </c>
-      <c r="AS44" s="45">
+      <c r="AT44" s="45">
         <v>14.1</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>115</v>
       </c>
@@ -9316,22 +9451,25 @@
         <v>64</v>
       </c>
       <c r="AO45" s="45">
+        <v>3.7389000000000001</v>
+      </c>
+      <c r="AP45" s="45">
         <v>23.6</v>
       </c>
-      <c r="AP45" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ45" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR45" s="45">
+      <c r="AR45" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS45" s="45">
         <v>8</v>
       </c>
-      <c r="AS45" s="45">
+      <c r="AT45" s="45">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>114</v>
       </c>
@@ -9453,22 +9591,25 @@
         <v>7.3</v>
       </c>
       <c r="AO46" s="45">
+        <v>5.4659000000000004</v>
+      </c>
+      <c r="AP46" s="45">
         <v>35.200000000000003</v>
       </c>
-      <c r="AP46" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ46" s="45">
+      <c r="AQ46" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR46" s="45">
         <v>4.2</v>
       </c>
-      <c r="AR46" s="45">
+      <c r="AS46" s="45">
         <v>17.7</v>
       </c>
-      <c r="AS46" s="45">
+      <c r="AT46" s="45">
         <v>14.3</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>113</v>
       </c>
@@ -9590,22 +9731,25 @@
         <v>64</v>
       </c>
       <c r="AO47" s="45">
+        <v>7.6612999999999998</v>
+      </c>
+      <c r="AP47" s="45">
         <v>23.2</v>
       </c>
-      <c r="AP47" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ47" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR47" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS47" s="45">
+      <c r="AS47" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT47" s="45">
         <v>12.4</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>112</v>
       </c>
@@ -9727,22 +9871,25 @@
         <v>64</v>
       </c>
       <c r="AO48" s="45">
+        <v>2.9944000000000002</v>
+      </c>
+      <c r="AP48" s="45">
         <v>28.8</v>
       </c>
-      <c r="AP48" s="45">
+      <c r="AQ48" s="45">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AQ48" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AR48" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS48" s="45">
+      <c r="AS48" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT48" s="45">
         <v>10.4</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>111</v>
       </c>
@@ -9864,22 +10011,25 @@
         <v>64</v>
       </c>
       <c r="AO49" s="45">
+        <v>5.7493999999999996</v>
+      </c>
+      <c r="AP49" s="45">
         <v>15.3</v>
       </c>
-      <c r="AP49" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ49" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR49" s="45">
+      <c r="AR49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS49" s="45">
         <v>16</v>
       </c>
-      <c r="AS49" s="45">
+      <c r="AT49" s="45">
         <v>9.9</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>110</v>
       </c>
@@ -10001,22 +10151,25 @@
         <v>3.5</v>
       </c>
       <c r="AO50" s="45">
+        <v>3.145</v>
+      </c>
+      <c r="AP50" s="45">
         <v>38.299999999999997</v>
       </c>
-      <c r="AP50" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ50" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR50" s="45">
+      <c r="AR50" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS50" s="45">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AS50" s="45">
+      <c r="AT50" s="45">
         <v>7.5</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>109</v>
       </c>
@@ -10138,22 +10291,25 @@
         <v>64</v>
       </c>
       <c r="AO51" s="45">
+        <v>6.3726000000000003</v>
+      </c>
+      <c r="AP51" s="45">
         <v>14.4</v>
       </c>
-      <c r="AP51" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ51" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR51" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS51" s="45">
+      <c r="AS51" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT51" s="45">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>108</v>
       </c>
@@ -10275,22 +10431,25 @@
         <v>64</v>
       </c>
       <c r="AO52" s="45">
+        <v>4.1067999999999998</v>
+      </c>
+      <c r="AP52" s="45">
         <v>17.8</v>
       </c>
-      <c r="AP52" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ52" s="45" t="s">
         <v>64</v>
       </c>
       <c r="AR52" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AS52" s="45">
+      <c r="AS52" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT52" s="45">
         <v>6.7</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>107</v>
       </c>
@@ -10412,22 +10571,25 @@
         <v>64</v>
       </c>
       <c r="AO53" s="45">
+        <v>10.465299999999999</v>
+      </c>
+      <c r="AP53" s="45">
         <v>26.2</v>
       </c>
-      <c r="AP53" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ53" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR53" s="45">
+      <c r="AR53" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS53" s="45">
         <v>11.8</v>
       </c>
-      <c r="AS53" s="45">
+      <c r="AT53" s="45">
         <v>18.7</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>106</v>
       </c>
@@ -10549,22 +10711,25 @@
         <v>64</v>
       </c>
       <c r="AO54" s="45">
+        <v>5.2919</v>
+      </c>
+      <c r="AP54" s="45">
         <v>39.799999999999997</v>
       </c>
-      <c r="AP54" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ54" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR54" s="45">
+      <c r="AR54" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS54" s="45">
         <v>12.6</v>
       </c>
-      <c r="AS54" s="45">
+      <c r="AT54" s="45">
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>105</v>
       </c>
@@ -10685,23 +10850,26 @@
       <c r="AN55" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AO55" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP55" s="45">
+      <c r="AO55" s="45">
+        <v>6.4835000000000003</v>
+      </c>
+      <c r="AP55" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ55" s="45">
         <v>15.2</v>
       </c>
-      <c r="AQ55" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR55" s="45">
+      <c r="AR55" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS55" s="45">
         <v>19.5</v>
       </c>
-      <c r="AS55" s="45">
+      <c r="AT55" s="45">
         <v>16.3</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>104</v>
       </c>
@@ -10823,22 +10991,25 @@
         <v>64</v>
       </c>
       <c r="AO56" s="45">
+        <v>7.86</v>
+      </c>
+      <c r="AP56" s="45">
         <v>39.4</v>
       </c>
-      <c r="AP56" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ56" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR56" s="45">
+      <c r="AR56" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS56" s="45">
         <v>13</v>
       </c>
-      <c r="AS56" s="45">
+      <c r="AT56" s="45">
         <v>15.8</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>103</v>
       </c>
@@ -10960,32 +11131,35 @@
         <v>64</v>
       </c>
       <c r="AO57" s="45">
+        <v>11.613200000000001</v>
+      </c>
+      <c r="AP57" s="45">
         <v>32.700000000000003</v>
       </c>
-      <c r="AP57" s="45">
+      <c r="AQ57" s="45">
         <v>24</v>
       </c>
-      <c r="AQ57" s="45">
-        <v>0</v>
-      </c>
       <c r="AR57" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS57" s="45">
         <v>33.299999999999997</v>
       </c>
-      <c r="AS57" s="45">
+      <c r="AT57" s="45">
         <v>27.4</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AB58" s="51"/>
       <c r="AC58" s="51"/>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B60" s="21"/>
       <c r="G60" s="21"/>
       <c r="L60" s="47"/>
       <c r="U60" s="22"/>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B61" s="36">
         <v>44952</v>
       </c>
@@ -11004,13 +11178,13 @@
       <c r="AH61" s="43"/>
       <c r="AI61" s="43"/>
       <c r="AJ61" s="43"/>
-      <c r="AO61" s="43"/>
       <c r="AP61" s="43"/>
       <c r="AQ61" s="43"/>
       <c r="AR61" s="43"/>
       <c r="AS61" s="43"/>
+      <c r="AT61" s="43"/>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B62" s="17" t="s">
         <v>61</v>
       </c>
@@ -11032,13 +11206,13 @@
       <c r="AH62" s="43"/>
       <c r="AI62" s="43"/>
       <c r="AJ62" s="43"/>
-      <c r="AO62" s="43"/>
       <c r="AP62" s="43"/>
       <c r="AQ62" s="43"/>
       <c r="AR62" s="43"/>
       <c r="AS62" s="43"/>
+      <c r="AT62" s="43"/>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B63" s="17" t="s">
         <v>62</v>
       </c>
@@ -11060,11 +11234,11 @@
       <c r="AH63" s="43"/>
       <c r="AI63" s="43"/>
       <c r="AJ63" s="43"/>
-      <c r="AO63" s="43"/>
       <c r="AP63" s="43"/>
       <c r="AQ63" s="43"/>
       <c r="AR63" s="43"/>
       <c r="AS63" s="43"/>
+      <c r="AT63" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26113,6 +26287,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003A6C5F82651BF147B7C9E4B3761618AB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b68ad2b4cbb1d4c00b5764baa4791088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4eab1d2f-0a6f-43b5-bd47-0cc182e7f81d" xmlns:ns3="18262a4b-7b39-4d27-b1ee-8cb22edac4a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20c901150ea431e28436f714a2271bce" ns2:_="" ns3:_="">
     <xsd:import namespace="4eab1d2f-0a6f-43b5-bd47-0cc182e7f81d"/>
@@ -26335,7 +26518,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="4eab1d2f-0a6f-43b5-bd47-0cc182e7f81d" xsi:nil="true"/>
@@ -26346,32 +26529,23 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54A02C79-545B-46E0-9D61-D46F3FC0D78A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6292575E-8E0B-4B70-BBE4-BBF3D81D31FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33F13424-6997-4A55-BB17-31487EE7D41C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CF42A5-3933-474A-B24D-2E86B0E96D31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6292575E-8E0B-4B70-BBE4-BBF3D81D31FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>